<commit_message>
completed research output, bugs fixed
</commit_message>
<xml_diff>
--- a/src/main/java/OrderTables404H.xlsx
+++ b/src/main/java/OrderTables404H.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F77A2C3-DAFF-4FB5-9551-996702D7F908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D41A96-202E-4B8B-9CCA-518BA6130B41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="25515" windowHeight="12630" tabRatio="300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3630" yWindow="345" windowWidth="10515" windowHeight="11355" tabRatio="560" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MAN18-64" sheetId="1" r:id="rId1"/>
@@ -1149,8 +1149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AY19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="AM7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="BA12" sqref="BA12"/>
@@ -4912,7 +4912,7 @@
   <dimension ref="A1:AY22"/>
   <sheetViews>
     <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="BH12" sqref="BH12"/>
@@ -7459,11 +7459,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AR17"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>